<commit_message>
add plotting to drawing RDM
</commit_message>
<xml_diff>
--- a/image_similarities/drawings_human_rated/instructions/instructions_kitchen.xlsx
+++ b/image_similarities/drawings_human_rated/instructions/instructions_kitchen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unigiessende-my.sharepoint.com/personal/gc2117_uni-giessen_de/Documents/Dokumente/GitHub/ratingTask_Micha/instructions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unigiessende-my.sharepoint.com/personal/gc2117_uni-giessen_de/Documents/Dokumente/GitHub/pep_wp4_beh/image_similarities/drawings_human_rated/instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{FE2E5AC3-5299-4B60-B42F-650764EE59E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAF8EB8-D976-4840-BD84-798511F59361}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{FE2E5AC3-5299-4B60-B42F-650764EE59E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{178C28ED-977D-4E56-A039-7DBD6F16C7A4}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="8680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
     <t>instructions/Slide5.jpg</t>
   </si>
   <si>
-    <t>instructions/Slide1.jpg</t>
+    <t>instructions/Slide2.jpg</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -645,12 +645,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -768,15 +765,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -798,16 +805,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>